<commit_message>
upload 2 of excel, 1 of word
</commit_message>
<xml_diff>
--- a/excels/【Excel】準2級②.xlsx
+++ b/excels/【Excel】準2級②.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.13.36\課題回収\おくむら(Web1B)\012コウヨウ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EA817A-2739-48C7-97B5-4FB59EAFA071}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069CA1D4-B2A8-49A7-98A8-44729F3D35C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="6" xr2:uid="{96D8D209-06D9-49DF-85C2-37D50E14455A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10845" windowHeight="11595" xr2:uid="{96D8D209-06D9-49DF-85C2-37D50E14455A}"/>
   </bookViews>
   <sheets>
     <sheet name="準2-5" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="199">
   <si>
     <t>贈答品請求額一覧表</t>
     <rPh sb="0" eb="3">
@@ -1542,6 +1542,30 @@
     <rPh sb="0" eb="1">
       <t>ウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>株数</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>支払額</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>受取額</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>時間</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>請求額</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ポイント</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1549,8 +1573,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0.0%"/>
+    <numFmt numFmtId="177" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
+    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1577,12 +1603,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="22">
@@ -1876,7 +1908,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1970,9 +2002,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1985,12 +2014,6 @@
     <xf numFmtId="38" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2036,13 +2059,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="0" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2361,18 +2459,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2F1F42-8D5E-4EC6-B8FF-63011781F4CD}">
-  <dimension ref="A1:P24"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.125" bestFit="1" customWidth="1"/>
@@ -2387,19 +2488,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
@@ -2928,112 +3029,54 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="70">
         <f>AVERAGE(H3:H11)</f>
         <v>17004.222222222223</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="70">
         <f>AVERAGE(J3:J11)</f>
         <v>1553.4444444444443</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="74">
         <f>AVERAGE(K3:K11)</f>
         <v>18557.666666666668</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="70">
         <f>MAX(H3:H11)</f>
         <v>26112</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C17" s="70">
         <f>MAX(J3:J11)</f>
         <v>2611</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="74">
         <f>MAX(K3:K11)</f>
         <v>28723</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="71">
         <f>MIN(H3:H11)</f>
         <v>10571</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="71">
         <f>MIN(J3:J11)</f>
         <v>946</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="75">
         <f>MIN(K3:K11)</f>
         <v>11628</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="B22" s="2" t="e">
-        <f>AVERAGE(B21:D21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C22" s="2" t="e">
-        <f t="shared" ref="C22:D22" si="8">AVERAGE(C21:E21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D22" s="9" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="B23" s="2">
-        <f>MAX(B21:D21)</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
-        <f t="shared" ref="C23:D23" si="9">MAX(C21:E21)</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="9">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="B24" s="12">
-        <f>MAX(B21,D21)</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="12">
-        <f t="shared" ref="C24:D24" si="10">MAX(C21,E21)</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="13">
-        <f t="shared" si="10"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3051,10 +3094,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A73604E-9B08-437A-BAEA-0C5406551274}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3073,19 +3119,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
@@ -3171,7 +3217,7 @@
       <c r="M3" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="N3" s="40">
+      <c r="N3" s="37">
         <v>0.187</v>
       </c>
     </row>
@@ -3218,7 +3264,7 @@
       <c r="M4" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="N4" s="40">
+      <c r="N4" s="37">
         <v>0.16400000000000001</v>
       </c>
     </row>
@@ -3265,7 +3311,7 @@
       <c r="M5" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="N5" s="41">
+      <c r="N5" s="38">
         <v>0.14099999999999999</v>
       </c>
     </row>
@@ -3520,63 +3566,63 @@
     <row r="13" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="30"/>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="70">
         <f>AVERAGE(D3:D10)</f>
         <v>484687.5</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="70">
         <f>AVERAGE(G3:G10)</f>
         <v>78181.625</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="74">
         <f>AVERAGE(I3:I10)</f>
         <v>71837.75</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="70">
         <f>MAX(D3:D10)</f>
         <v>567375</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="70">
         <f>MAX(G3:G10)</f>
         <v>96468</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="74">
         <f>MAX(I3:I10)</f>
         <v>80413</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17" s="71">
         <f>MIN(D3:D10)</f>
         <v>411625</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="71">
         <f>MIN(G3:G10)</f>
         <v>58039</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="75">
         <f>MIN(I3:I10)</f>
         <v>62865</v>
       </c>
@@ -3615,13 +3661,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
@@ -3667,7 +3713,7 @@
       <c r="L3" s="16">
         <v>3000</v>
       </c>
-      <c r="M3" s="40">
+      <c r="M3" s="37">
         <v>0.13600000000000001</v>
       </c>
     </row>
@@ -3692,7 +3738,7 @@
       <c r="L4" s="16">
         <v>2000</v>
       </c>
-      <c r="M4" s="40">
+      <c r="M4" s="37">
         <v>0.127</v>
       </c>
     </row>
@@ -3717,7 +3763,7 @@
       <c r="L5" s="19">
         <v>1</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="38">
         <v>0.11799999999999999</v>
       </c>
     </row>
@@ -3756,25 +3802,25 @@
         <f>AVERAGE(C3:C6)</f>
         <v>2437.5</v>
       </c>
-      <c r="D8" s="42"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="28">
         <f t="shared" ref="E8" si="2">AVERAGE(E3:E6)</f>
         <v>312.75</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -4188,20 +4234,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
@@ -4293,7 +4339,7 @@
       <c r="N3" s="16">
         <v>101</v>
       </c>
-      <c r="O3" s="45" t="s">
+      <c r="O3" s="42" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4343,7 +4389,7 @@
       <c r="N4" s="16">
         <v>102</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="42" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4393,7 +4439,7 @@
       <c r="N5" s="19">
         <v>103</v>
       </c>
-      <c r="O5" s="46" t="s">
+      <c r="O5" s="43" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4528,10 +4574,10 @@
         <f t="shared" si="5"/>
         <v>##</v>
       </c>
-      <c r="N8" s="43" t="s">
+      <c r="N8" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="O8" s="44">
+      <c r="O8" s="41">
         <v>258700</v>
       </c>
     </row>
@@ -4720,7 +4766,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="35" t="s">
         <v>168</v>
       </c>
       <c r="B16" s="29">
@@ -4731,13 +4777,13 @@
         <f>AVERAGE(F3:F11)</f>
         <v>7279.7777777777774</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="32">
         <f>AVERAGE(G3:G11)</f>
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="35" t="s">
         <v>170</v>
       </c>
       <c r="B17" s="29">
@@ -4748,24 +4794,24 @@
         <f>MAX(F3:F11)</f>
         <v>9368</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="32">
         <f>MAX(G3:G11)</f>
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="33">
         <f>MIN(E3:E11)</f>
         <v>2193000</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="33">
         <f>MIN(F3:F11)</f>
         <v>5139</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="34">
         <f>MIN(G3:G11)</f>
         <v>9</v>
       </c>
@@ -4807,18 +4853,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
@@ -4904,7 +4950,7 @@
       <c r="M3" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N3" s="47">
+      <c r="N3" s="44">
         <v>105</v>
       </c>
     </row>
@@ -4951,7 +4997,7 @@
       <c r="M4" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="N4" s="47">
+      <c r="N4" s="44">
         <v>13</v>
       </c>
     </row>
@@ -4998,7 +5044,7 @@
       <c r="M5" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="N5" s="47">
+      <c r="N5" s="44">
         <v>90</v>
       </c>
     </row>
@@ -5045,7 +5091,7 @@
       <c r="M6" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="N6" s="48">
+      <c r="N6" s="45">
         <v>9</v>
       </c>
     </row>
@@ -5250,7 +5296,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="35" t="s">
         <v>168</v>
       </c>
       <c r="B15" s="25">
@@ -5267,7 +5313,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="35" t="s">
         <v>170</v>
       </c>
       <c r="B16" s="25">
@@ -5284,7 +5330,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="36" t="s">
         <v>181</v>
       </c>
       <c r="B17" s="26">
@@ -5317,7 +5363,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5335,13 +5381,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
@@ -5359,10 +5405,10 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="47" t="s">
         <v>190</v>
       </c>
-      <c r="L2" s="51">
+      <c r="L2" s="48">
         <v>145.44999999999999</v>
       </c>
     </row>
@@ -5373,7 +5419,7 @@
       <c r="B3" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="46">
         <v>21436</v>
       </c>
       <c r="D3" s="25">
@@ -5391,7 +5437,7 @@
       <c r="B4" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="46">
         <v>22695</v>
       </c>
       <c r="D4" s="25">
@@ -5409,7 +5455,7 @@
       <c r="B5" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="46">
         <v>19243</v>
       </c>
       <c r="D5" s="25">
@@ -5427,7 +5473,7 @@
       <c r="B6" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="46">
         <v>23147</v>
       </c>
       <c r="D6" s="25">
@@ -5450,28 +5496,28 @@
       <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C8" s="50">
         <f>SUM(C3:C6)</f>
         <v>86521</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="33">
         <f>SUM(D3:D6)</f>
         <v>1796</v>
       </c>
       <c r="E8" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -5850,297 +5896,628 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55BF62A-37B7-4D13-8933-ABFA6EF8BFC6}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="9" style="52"/>
+    <col min="1" max="1" width="6" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.125" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="5.25" style="49" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.125" style="49" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="73" t="s">
         <v>124</v>
       </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="61" t="s">
         <v>128</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="61" t="s">
         <v>130</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="62" t="s">
         <v>54</v>
       </c>
       <c r="N2" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="52" t="s">
+      <c r="O2" s="53" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A3" s="52">
+      <c r="A3" s="54">
         <v>11</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="52">
+      <c r="C3" s="51">
         <v>102</v>
       </c>
-      <c r="D3" s="52" t="str">
-        <f>VLOOKUP(C3,$N$3:$O$6,2,FALSE)</f>
+      <c r="D3" s="51" t="str">
+        <f t="shared" ref="D3:D11" si="0">VLOOKUP(C3,$N$3:$O$6,2,FALSE)</f>
         <v>中央薬品</v>
       </c>
-      <c r="E3" s="52">
+      <c r="E3" s="25">
         <v>300</v>
       </c>
-      <c r="G3" s="52">
+      <c r="F3" s="25">
+        <v>3620</v>
+      </c>
+      <c r="G3" s="25">
         <v>3890</v>
       </c>
-      <c r="N3" s="52">
+      <c r="H3" s="25">
+        <f t="shared" ref="H3:H11" si="1">ROUNDUP(F3*E3*(1+$O$9),0)</f>
+        <v>1087955</v>
+      </c>
+      <c r="I3" s="25">
+        <f t="shared" ref="I3:I11" si="2">INT(G3*E3*(1-$O$10))</f>
+        <v>1165366</v>
+      </c>
+      <c r="J3" s="25">
+        <f t="shared" ref="J3:J11" si="3">I3-H3</f>
+        <v>77411</v>
+      </c>
+      <c r="K3" s="51">
+        <f t="shared" ref="K3:K11" si="4">RANK(I3,$I$3:$I$11,1)</f>
+        <v>3</v>
+      </c>
+      <c r="L3" s="55" t="str">
+        <f t="shared" ref="L3:L11" si="5">IF(OR(I3&lt;=1200000,J3&gt;=70000),"A", "B")</f>
+        <v>A</v>
+      </c>
+      <c r="N3" s="54">
         <v>101</v>
       </c>
-      <c r="O3" s="52" t="s">
+      <c r="O3" s="55" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A4" s="52">
+      <c r="A4" s="54">
         <v>12</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="51">
         <v>104</v>
       </c>
-      <c r="D4" s="52" t="str">
-        <f t="shared" ref="D4:D11" si="0">VLOOKUP(C4,$N$3:$O$6,2,FALSE)</f>
+      <c r="D4" s="51" t="str">
+        <f t="shared" si="0"/>
         <v>新生電気</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="25">
         <v>500</v>
       </c>
-      <c r="G4" s="52">
+      <c r="F4" s="25">
+        <v>2730</v>
+      </c>
+      <c r="G4" s="25">
         <v>2890</v>
       </c>
-      <c r="N4" s="52">
+      <c r="H4" s="25">
+        <f t="shared" si="1"/>
+        <v>1367457</v>
+      </c>
+      <c r="I4" s="25">
+        <f t="shared" si="2"/>
+        <v>1442977</v>
+      </c>
+      <c r="J4" s="25">
+        <f t="shared" si="3"/>
+        <v>75520</v>
+      </c>
+      <c r="K4" s="51">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="L4" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v>A</v>
+      </c>
+      <c r="N4" s="54">
         <v>102</v>
       </c>
-      <c r="O4" s="52" t="s">
+      <c r="O4" s="55" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A5" s="52">
+      <c r="A5" s="54">
+        <v>16</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="51">
+        <v>104</v>
+      </c>
+      <c r="D5" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>新生電気</v>
+      </c>
+      <c r="E5" s="25">
+        <v>600</v>
+      </c>
+      <c r="F5" s="25">
+        <v>2860</v>
+      </c>
+      <c r="G5" s="25">
+        <v>2980</v>
+      </c>
+      <c r="H5" s="25">
+        <f t="shared" si="1"/>
+        <v>1719089</v>
+      </c>
+      <c r="I5" s="25">
+        <f t="shared" si="2"/>
+        <v>1785496</v>
+      </c>
+      <c r="J5" s="25">
+        <f t="shared" si="3"/>
+        <v>66407</v>
+      </c>
+      <c r="K5" s="51">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="L5" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v>B</v>
+      </c>
+      <c r="N5" s="54">
+        <v>103</v>
+      </c>
+      <c r="O5" s="55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="54">
         <v>13</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C6" s="51">
         <v>101</v>
       </c>
-      <c r="D5" s="52" t="str">
+      <c r="D6" s="51" t="str">
         <f t="shared" si="0"/>
         <v>北陸工業</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E6" s="25">
         <v>2500</v>
       </c>
-      <c r="G5" s="52">
+      <c r="F6" s="25">
+        <v>685</v>
+      </c>
+      <c r="G6" s="25">
         <v>705</v>
       </c>
-      <c r="N5" s="52">
+      <c r="H6" s="25">
+        <f t="shared" si="1"/>
+        <v>1715583</v>
+      </c>
+      <c r="I6" s="25">
+        <f t="shared" si="2"/>
+        <v>1760032</v>
+      </c>
+      <c r="J6" s="25">
+        <f t="shared" si="3"/>
+        <v>44449</v>
+      </c>
+      <c r="K6" s="51">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="L6" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v>B</v>
+      </c>
+      <c r="N6" s="56">
+        <v>104</v>
+      </c>
+      <c r="O6" s="57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="54">
+        <v>19</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="51">
+        <v>102</v>
+      </c>
+      <c r="D7" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>中央薬品</v>
+      </c>
+      <c r="E7" s="25">
+        <v>400</v>
+      </c>
+      <c r="F7" s="25">
+        <v>3570</v>
+      </c>
+      <c r="G7" s="25">
+        <v>3690</v>
+      </c>
+      <c r="H7" s="25">
+        <f t="shared" si="1"/>
+        <v>1430571</v>
+      </c>
+      <c r="I7" s="25">
+        <f t="shared" si="2"/>
+        <v>1473933</v>
+      </c>
+      <c r="J7" s="25">
+        <f t="shared" si="3"/>
+        <v>43362</v>
+      </c>
+      <c r="K7" s="51">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="L7" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="54">
+        <v>14</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="51">
         <v>103</v>
       </c>
-      <c r="O5" s="52" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A6" s="52">
-        <v>14</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="52">
-        <v>103</v>
-      </c>
-      <c r="D6" s="52" t="str">
+      <c r="D8" s="51" t="str">
         <f t="shared" si="0"/>
         <v>井上証券</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E8" s="25">
         <v>3000</v>
       </c>
-      <c r="G6" s="52">
+      <c r="F8" s="25">
+        <v>564</v>
+      </c>
+      <c r="G8" s="25">
         <v>578</v>
       </c>
-      <c r="N6" s="52">
-        <v>104</v>
-      </c>
-      <c r="O6" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A7" s="52">
+      <c r="H8" s="25">
+        <f t="shared" si="1"/>
+        <v>1695046</v>
+      </c>
+      <c r="I8" s="25">
+        <f t="shared" si="2"/>
+        <v>1731572</v>
+      </c>
+      <c r="J8" s="25">
+        <f t="shared" si="3"/>
+        <v>36526</v>
+      </c>
+      <c r="K8" s="51">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="L8" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" s="54">
         <v>15</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C9" s="51">
         <v>101</v>
       </c>
-      <c r="D7" s="52" t="str">
+      <c r="D9" s="51" t="str">
         <f t="shared" si="0"/>
         <v>北陸工業</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E9" s="25">
         <v>1500</v>
       </c>
-      <c r="G7" s="52">
+      <c r="F9" s="25">
+        <v>672</v>
+      </c>
+      <c r="G9" s="25">
         <v>697</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A8" s="52">
-        <v>16</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="52">
-        <v>104</v>
-      </c>
-      <c r="D8" s="52" t="str">
+      <c r="H9" s="25">
+        <f t="shared" si="1"/>
+        <v>1009815</v>
+      </c>
+      <c r="I9" s="25">
+        <f t="shared" si="2"/>
+        <v>1044036</v>
+      </c>
+      <c r="J9" s="25">
+        <f t="shared" si="3"/>
+        <v>34221</v>
+      </c>
+      <c r="K9" s="51">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L9" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v>A</v>
+      </c>
+      <c r="N9" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="O9" s="58">
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="54">
+        <v>18</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="51">
+        <v>101</v>
+      </c>
+      <c r="D10" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>新生電気</v>
-      </c>
-      <c r="E8" s="52">
-        <v>600</v>
-      </c>
-      <c r="G8" s="52">
-        <v>2980</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A9" s="52">
+        <v>北陸工業</v>
+      </c>
+      <c r="E10" s="25">
+        <v>2000</v>
+      </c>
+      <c r="F10" s="25">
+        <v>714</v>
+      </c>
+      <c r="G10" s="25">
+        <v>708</v>
+      </c>
+      <c r="H10" s="25">
+        <f t="shared" si="1"/>
+        <v>1430571</v>
+      </c>
+      <c r="I10" s="25">
+        <f t="shared" si="2"/>
+        <v>1414017</v>
+      </c>
+      <c r="J10" s="25">
+        <f t="shared" si="3"/>
+        <v>-16554</v>
+      </c>
+      <c r="K10" s="51">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="L10" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v>B</v>
+      </c>
+      <c r="N10" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="O10" s="59">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="54">
         <v>17</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B11" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="52">
+      <c r="C11" s="51">
         <v>103</v>
       </c>
-      <c r="D9" s="52" t="str">
+      <c r="D11" s="51" t="str">
         <f t="shared" si="0"/>
         <v>井上証券</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E11" s="25">
         <v>2000</v>
       </c>
-      <c r="G9" s="52">
+      <c r="F11" s="25">
+        <v>572</v>
+      </c>
+      <c r="G11" s="25">
         <v>563</v>
       </c>
-      <c r="N9" s="52" t="s">
-        <v>191</v>
-      </c>
-      <c r="O9" s="55">
-        <v>1.8E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A10" s="52">
-        <v>18</v>
-      </c>
-      <c r="B10" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="52">
-        <v>101</v>
-      </c>
-      <c r="D10" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v>北陸工業</v>
-      </c>
-      <c r="E10" s="52">
-        <v>2000</v>
-      </c>
-      <c r="G10" s="52">
-        <v>708</v>
-      </c>
-      <c r="N10" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="O10" s="55">
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A11" s="52">
-        <v>19</v>
-      </c>
-      <c r="B11" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="52">
-        <v>102</v>
-      </c>
-      <c r="D11" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v>中央薬品</v>
-      </c>
-      <c r="E11" s="52">
-        <v>400</v>
-      </c>
-      <c r="G11" s="52">
-        <v>3690</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B13" s="52" t="s">
+      <c r="H11" s="25">
+        <f t="shared" si="1"/>
+        <v>1146060</v>
+      </c>
+      <c r="I11" s="25">
+        <f t="shared" si="2"/>
+        <v>1124423</v>
+      </c>
+      <c r="J11" s="25">
+        <f t="shared" si="3"/>
+        <v>-21637</v>
+      </c>
+      <c r="K11" s="51">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L11" s="55" t="str">
+        <f t="shared" si="5"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A12" s="54"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="55"/>
+    </row>
+    <row r="13" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="56"/>
+      <c r="B13" s="63" t="s">
         <v>21</v>
       </c>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26">
+        <f>SUM(H3:H11)</f>
+        <v>12602147</v>
+      </c>
+      <c r="I13" s="26">
+        <f t="shared" ref="I13:J13" si="6">SUM(I3:I11)</f>
+        <v>12941852</v>
+      </c>
+      <c r="J13" s="26">
+        <f t="shared" si="6"/>
+        <v>339705</v>
+      </c>
+      <c r="K13" s="64"/>
+      <c r="L13" s="57"/>
+    </row>
+    <row r="15" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="30"/>
+      <c r="B16" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="29">
+        <f>AVERAGE(E3:E11)</f>
+        <v>1422.2222222222222</v>
+      </c>
+      <c r="C17" s="65">
+        <f>AVERAGE(H3:H11)</f>
+        <v>1400238.5555555555</v>
+      </c>
+      <c r="D17" s="66">
+        <f>AVERAGE(I3:I11)</f>
+        <v>1437983.5555555555</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="29">
+        <f>MAX(E3:E11)</f>
+        <v>3000</v>
+      </c>
+      <c r="C18" s="65">
+        <f>MAX(H3:H11)</f>
+        <v>1719089</v>
+      </c>
+      <c r="D18" s="66">
+        <f>MAX(I3:I11)</f>
+        <v>1785496</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="33">
+        <f>MIN(E3:E11)</f>
+        <v>300</v>
+      </c>
+      <c r="C19" s="67">
+        <f>MIN(H3:H11)</f>
+        <v>1009815</v>
+      </c>
+      <c r="D19" s="67">
+        <f>MIN(I3:I11)</f>
+        <v>1044036</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A3:L11">
+    <sortCondition descending="1" ref="J2"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6149,103 +6526,599 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB72ED9-4144-4ADE-B2C9-B80826544FF2}">
-  <dimension ref="A1:L12"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.375" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="72" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+    </row>
+    <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A3" s="8">
+        <v>101</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
+      <c r="C3" s="2">
+        <v>14</v>
+      </c>
+      <c r="D3" s="25">
+        <f t="shared" ref="D3:D10" si="0">VLOOKUP(C3,$N$4:$O$7,2,FALSE)</f>
+        <v>13100</v>
+      </c>
+      <c r="E3" s="25">
+        <v>9</v>
+      </c>
+      <c r="F3" s="25">
+        <f t="shared" ref="F3:F10" si="1">IF(E3&lt;=10,0,D3/10*(E3-10)*0.5)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="25">
+        <f t="shared" ref="G3:G10" si="2">D3+F3</f>
+        <v>13100</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H10" si="3">IF(G3&gt;=17000,5%,IF(G3&gt;=13000,4.2%,3.4%))</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I3" s="25">
+        <f t="shared" ref="I3:I10" si="4">INT(G3*H3)</f>
+        <v>550</v>
+      </c>
+      <c r="J3" s="25">
+        <f t="shared" ref="J3:J10" si="5">G3-I3</f>
+        <v>12550</v>
+      </c>
+      <c r="K3" s="25">
+        <f t="shared" ref="K3:K10" si="6">ROUNDUP(J3*1.3%,0)</f>
+        <v>164</v>
+      </c>
+      <c r="L3" s="9" t="str">
+        <f t="shared" ref="L3:L10" si="7">IF(OR(E3&lt;=10,J3&lt;=12000),"G","")</f>
+        <v>G</v>
+      </c>
+      <c r="N3" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" s="8">
+        <v>103</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="2">
+        <v>11</v>
+      </c>
+      <c r="D4" s="25">
+        <f t="shared" si="0"/>
+        <v>12400</v>
+      </c>
+      <c r="E4" s="25">
+        <v>10</v>
+      </c>
+      <c r="F4" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" si="2"/>
+        <v>12400</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="3"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I4" s="25">
+        <f t="shared" si="4"/>
+        <v>421</v>
+      </c>
+      <c r="J4" s="25">
+        <f t="shared" si="5"/>
+        <v>11979</v>
+      </c>
+      <c r="K4" s="25">
+        <f t="shared" si="6"/>
         <v>156</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
+      <c r="L4" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v>G</v>
+      </c>
+      <c r="N4" s="8">
+        <v>11</v>
+      </c>
+      <c r="O4" s="27">
+        <v>12400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" s="8">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12</v>
+      </c>
+      <c r="D5" s="25">
+        <f t="shared" si="0"/>
+        <v>11300</v>
+      </c>
+      <c r="E5" s="25">
+        <v>11</v>
+      </c>
+      <c r="F5" s="25">
+        <f t="shared" si="1"/>
+        <v>565</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="2"/>
+        <v>11865</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="3"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I5" s="25">
+        <f t="shared" si="4"/>
+        <v>403</v>
+      </c>
+      <c r="J5" s="25">
+        <f t="shared" si="5"/>
+        <v>11462</v>
+      </c>
+      <c r="K5" s="25">
+        <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="L5" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v>G</v>
+      </c>
+      <c r="N5" s="8">
+        <v>12</v>
+      </c>
+      <c r="O5" s="27">
+        <v>11300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6" s="8">
+        <v>105</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="2">
+        <v>12</v>
+      </c>
+      <c r="D6" s="25">
+        <f t="shared" si="0"/>
+        <v>11300</v>
+      </c>
+      <c r="E6" s="25">
+        <v>13</v>
+      </c>
+      <c r="F6" s="25">
+        <f t="shared" si="1"/>
+        <v>1695</v>
+      </c>
+      <c r="G6" s="25">
+        <f t="shared" si="2"/>
+        <v>12995</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="3"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I6" s="25">
+        <f t="shared" si="4"/>
+        <v>441</v>
+      </c>
+      <c r="J6" s="25">
+        <f t="shared" si="5"/>
+        <v>12554</v>
+      </c>
+      <c r="K6" s="25">
+        <f t="shared" si="6"/>
+        <v>164</v>
+      </c>
+      <c r="L6" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N6" s="8">
+        <v>13</v>
+      </c>
+      <c r="O6" s="27">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="8">
+        <v>106</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="2">
+        <v>14</v>
+      </c>
+      <c r="D7" s="25">
+        <f t="shared" si="0"/>
+        <v>13100</v>
+      </c>
+      <c r="E7" s="25">
+        <v>17</v>
+      </c>
+      <c r="F7" s="25">
+        <f t="shared" si="1"/>
+        <v>4585</v>
+      </c>
+      <c r="G7" s="25">
+        <f t="shared" si="2"/>
+        <v>17685</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="I7" s="25">
+        <f t="shared" si="4"/>
+        <v>884</v>
+      </c>
+      <c r="J7" s="25">
+        <f t="shared" si="5"/>
+        <v>16801</v>
+      </c>
+      <c r="K7" s="25">
+        <f t="shared" si="6"/>
+        <v>219</v>
+      </c>
+      <c r="L7" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N7" s="10">
+        <v>14</v>
+      </c>
+      <c r="O7" s="28">
+        <v>13100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="8">
+        <v>107</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="2">
+        <v>11</v>
+      </c>
+      <c r="D8" s="25">
+        <f t="shared" si="0"/>
+        <v>12400</v>
+      </c>
+      <c r="E8" s="25">
+        <v>18</v>
+      </c>
+      <c r="F8" s="25">
+        <f t="shared" si="1"/>
+        <v>4960</v>
+      </c>
+      <c r="G8" s="25">
+        <f t="shared" si="2"/>
+        <v>17360</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="I8" s="25">
+        <f t="shared" si="4"/>
+        <v>868</v>
+      </c>
+      <c r="J8" s="25">
+        <f t="shared" si="5"/>
+        <v>16492</v>
+      </c>
+      <c r="K8" s="25">
+        <f t="shared" si="6"/>
+        <v>215</v>
+      </c>
+      <c r="L8" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" s="8">
+        <v>102</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="2">
+        <v>13</v>
+      </c>
+      <c r="D9" s="25">
+        <f t="shared" si="0"/>
+        <v>10200</v>
+      </c>
+      <c r="E9" s="25">
+        <v>20</v>
+      </c>
+      <c r="F9" s="25">
+        <f t="shared" si="1"/>
+        <v>5100</v>
+      </c>
+      <c r="G9" s="25">
+        <f t="shared" si="2"/>
+        <v>15300</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="3"/>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I9" s="25">
+        <f t="shared" si="4"/>
+        <v>642</v>
+      </c>
+      <c r="J9" s="25">
+        <f t="shared" si="5"/>
+        <v>14658</v>
+      </c>
+      <c r="K9" s="25">
+        <f t="shared" si="6"/>
+        <v>191</v>
+      </c>
+      <c r="L9" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" s="8">
+        <v>104</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B12" t="s">
+      <c r="C10" s="2">
+        <v>13</v>
+      </c>
+      <c r="D10" s="25">
+        <f t="shared" si="0"/>
+        <v>10200</v>
+      </c>
+      <c r="E10" s="25">
         <v>21</v>
       </c>
+      <c r="F10" s="25">
+        <f t="shared" si="1"/>
+        <v>5610</v>
+      </c>
+      <c r="G10" s="25">
+        <f t="shared" si="2"/>
+        <v>15810</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="3"/>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I10" s="25">
+        <f t="shared" si="4"/>
+        <v>664</v>
+      </c>
+      <c r="J10" s="25">
+        <f t="shared" si="5"/>
+        <v>15146</v>
+      </c>
+      <c r="K10" s="25">
+        <f t="shared" si="6"/>
+        <v>197</v>
+      </c>
+      <c r="L10" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="8"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="26">
+        <f>SUM(D3:D10)</f>
+        <v>94000</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26">
+        <f t="shared" ref="F12:K12" si="8">SUM(F3:F10)</f>
+        <v>22515</v>
+      </c>
+      <c r="G12" s="26">
+        <f t="shared" si="8"/>
+        <v>116515</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="26">
+        <f t="shared" si="8"/>
+        <v>4873</v>
+      </c>
+      <c r="J12" s="26">
+        <f t="shared" si="8"/>
+        <v>111642</v>
+      </c>
+      <c r="K12" s="26">
+        <f t="shared" si="8"/>
+        <v>1456</v>
+      </c>
+      <c r="L12" s="13"/>
+    </row>
+    <row r="13" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="30"/>
+      <c r="B14" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A15" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="29">
+        <f>AVERAGE(E3:E10)</f>
+        <v>14.875</v>
+      </c>
+      <c r="C15" s="76">
+        <f>AVERAGE(J3:J10)</f>
+        <v>13955.25</v>
+      </c>
+      <c r="D15" s="68">
+        <f>AVERAGE(K3:K10)</f>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="29">
+        <f>MAX(E3:E10)</f>
+        <v>21</v>
+      </c>
+      <c r="C16" s="76">
+        <f>MAX(J3:J10)</f>
+        <v>16801</v>
+      </c>
+      <c r="D16" s="68">
+        <f>MAX(K3:K10)</f>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="33">
+        <f>MIN(E3:E10)</f>
+        <v>9</v>
+      </c>
+      <c r="C17" s="77">
+        <f>MIN(J3:J10)</f>
+        <v>11462</v>
+      </c>
+      <c r="D17" s="69">
+        <f>MIN(K3:K10)</f>
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A3:L10">
+    <sortCondition ref="E2"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>